<commit_message>
separation between Location and core
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/bind_excel_cell.xlsx
+++ b/src/test/resources/excel/bind_excel_cell.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>A1</t>
     <phoneticPr fontId="1"/>
@@ -36,7 +36,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>${A2}</t>
+    <t>C1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${C1_1}-${C1_2}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${B1}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -431,28 +439,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.7109375" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>